<commit_message>
Opcode implementation table updated
</commit_message>
<xml_diff>
--- a/other/op_codes_implementations.xlsx
+++ b/other/op_codes_implementations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="0" windowWidth="25940" windowHeight="16080" tabRatio="500"/>
+    <workbookView xWindow="1000" yWindow="360" windowWidth="25940" windowHeight="16080" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Main Codes" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8200" uniqueCount="1317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8648" uniqueCount="1323">
   <si>
     <t>0</t>
   </si>
@@ -4024,6 +4024,24 @@
   </si>
   <si>
     <t>inc</t>
+  </si>
+  <si>
+    <t>checkBit</t>
+  </si>
+  <si>
+    <t>setBit</t>
+  </si>
+  <si>
+    <t>rotateLeft</t>
+  </si>
+  <si>
+    <t>rotateRight</t>
+  </si>
+  <si>
+    <t>rotateLeftThroughFlag</t>
+  </si>
+  <si>
+    <t>rotateRightThroughFlag</t>
   </si>
 </sst>
 </file>
@@ -4072,8 +4090,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4093,7 +4125,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4101,6 +4133,13 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4108,6 +4147,13 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4447,7 +4493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R256"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -17502,10 +17548,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P256"/>
+  <dimension ref="A1:R256"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="R26" sqref="R26:R32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -17528,7 +17574,7 @@
     <col min="16" max="16" width="36.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -17574,8 +17620,14 @@
       <c r="P1" s="1" t="s">
         <v>1034</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
+      <c r="Q1" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -17621,8 +17673,14 @@
       <c r="P2" s="1" t="s">
         <v>1034</v>
       </c>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="Q2" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -17668,8 +17726,14 @@
       <c r="P3" s="1" t="s">
         <v>1034</v>
       </c>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="Q3" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -17715,8 +17779,14 @@
       <c r="P4" s="1" t="s">
         <v>1034</v>
       </c>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="Q4" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -17762,8 +17832,14 @@
       <c r="P5" s="1" t="s">
         <v>1034</v>
       </c>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="Q5" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6" s="1" t="s">
         <v>40</v>
       </c>
@@ -17809,8 +17885,14 @@
       <c r="P6" s="1" t="s">
         <v>1034</v>
       </c>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="Q6" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7" s="1" t="s">
         <v>47</v>
       </c>
@@ -17856,8 +17938,14 @@
       <c r="P7" s="1" t="s">
         <v>1034</v>
       </c>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="Q7" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8" s="1" t="s">
         <v>53</v>
       </c>
@@ -17903,8 +17991,14 @@
       <c r="P8" s="1" t="s">
         <v>1034</v>
       </c>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="Q8" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
@@ -17950,8 +18044,14 @@
       <c r="P9" s="1" t="s">
         <v>1044</v>
       </c>
-    </row>
-    <row r="10" spans="1:16">
+      <c r="Q9" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10" s="1" t="s">
         <v>67</v>
       </c>
@@ -17997,8 +18097,14 @@
       <c r="P10" s="1" t="s">
         <v>1044</v>
       </c>
-    </row>
-    <row r="11" spans="1:16">
+      <c r="Q10" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11" s="1" t="s">
         <v>75</v>
       </c>
@@ -18044,8 +18150,14 @@
       <c r="P11" s="1" t="s">
         <v>1044</v>
       </c>
-    </row>
-    <row r="12" spans="1:16">
+      <c r="Q11" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12" s="1" t="s">
         <v>80</v>
       </c>
@@ -18091,8 +18203,14 @@
       <c r="P12" s="1" t="s">
         <v>1044</v>
       </c>
-    </row>
-    <row r="13" spans="1:16">
+      <c r="Q12" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -18138,8 +18256,14 @@
       <c r="P13" s="1" t="s">
         <v>1044</v>
       </c>
-    </row>
-    <row r="14" spans="1:16">
+      <c r="Q13" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14" s="1" t="s">
         <v>89</v>
       </c>
@@ -18185,8 +18309,14 @@
       <c r="P14" s="1" t="s">
         <v>1044</v>
       </c>
-    </row>
-    <row r="15" spans="1:16">
+      <c r="Q14" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15" s="1" t="s">
         <v>94</v>
       </c>
@@ -18232,8 +18362,14 @@
       <c r="P15" s="1" t="s">
         <v>1044</v>
       </c>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="Q15" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16" s="1" t="s">
         <v>99</v>
       </c>
@@ -18279,8 +18415,14 @@
       <c r="P16" s="1" t="s">
         <v>1044</v>
       </c>
-    </row>
-    <row r="17" spans="1:16">
+      <c r="Q16" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
       <c r="A17" s="1" t="s">
         <v>105</v>
       </c>
@@ -18326,8 +18468,14 @@
       <c r="P17" s="1" t="s">
         <v>1054</v>
       </c>
-    </row>
-    <row r="18" spans="1:16">
+      <c r="Q17" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
       <c r="A18" s="1" t="s">
         <v>110</v>
       </c>
@@ -18373,8 +18521,14 @@
       <c r="P18" s="1" t="s">
         <v>1054</v>
       </c>
-    </row>
-    <row r="19" spans="1:16">
+      <c r="Q18" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
       <c r="A19" s="1" t="s">
         <v>114</v>
       </c>
@@ -18420,8 +18574,14 @@
       <c r="P19" s="1" t="s">
         <v>1054</v>
       </c>
-    </row>
-    <row r="20" spans="1:16">
+      <c r="Q19" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
       <c r="A20" s="1" t="s">
         <v>118</v>
       </c>
@@ -18467,8 +18627,14 @@
       <c r="P20" s="1" t="s">
         <v>1054</v>
       </c>
-    </row>
-    <row r="21" spans="1:16">
+      <c r="Q20" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
       <c r="A21" s="1" t="s">
         <v>66</v>
       </c>
@@ -18514,8 +18680,14 @@
       <c r="P21" s="1" t="s">
         <v>1054</v>
       </c>
-    </row>
-    <row r="22" spans="1:16">
+      <c r="Q21" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
       <c r="A22" s="1" t="s">
         <v>124</v>
       </c>
@@ -18561,8 +18733,14 @@
       <c r="P22" s="1" t="s">
         <v>1054</v>
       </c>
-    </row>
-    <row r="23" spans="1:16">
+      <c r="Q22" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
       <c r="A23" s="1" t="s">
         <v>127</v>
       </c>
@@ -18608,8 +18786,14 @@
       <c r="P23" s="1" t="s">
         <v>1054</v>
       </c>
-    </row>
-    <row r="24" spans="1:16">
+      <c r="Q23" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18">
       <c r="A24" s="1" t="s">
         <v>130</v>
       </c>
@@ -18655,8 +18839,14 @@
       <c r="P24" s="1" t="s">
         <v>1054</v>
       </c>
-    </row>
-    <row r="25" spans="1:16">
+      <c r="Q24" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18">
       <c r="A25" s="1" t="s">
         <v>134</v>
       </c>
@@ -18702,8 +18892,14 @@
       <c r="P25" s="1" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="26" spans="1:16">
+      <c r="Q25" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18">
       <c r="A26" s="1" t="s">
         <v>140</v>
       </c>
@@ -18749,8 +18945,14 @@
       <c r="P26" s="1" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="27" spans="1:16">
+      <c r="Q26" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R26" s="1" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18">
       <c r="A27" s="1" t="s">
         <v>143</v>
       </c>
@@ -18796,8 +18998,14 @@
       <c r="P27" s="1" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="28" spans="1:16">
+      <c r="Q27" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R27" s="1" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18">
       <c r="A28" s="1" t="s">
         <v>147</v>
       </c>
@@ -18843,8 +19051,14 @@
       <c r="P28" s="1" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="29" spans="1:16">
+      <c r="Q28" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R28" s="1" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18">
       <c r="A29" s="1" t="s">
         <v>151</v>
       </c>
@@ -18890,8 +19104,14 @@
       <c r="P29" s="1" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="30" spans="1:16">
+      <c r="Q29" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R29" s="1" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18">
       <c r="A30" s="1" t="s">
         <v>156</v>
       </c>
@@ -18937,8 +19157,14 @@
       <c r="P30" s="1" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="31" spans="1:16">
+      <c r="Q30" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R30" s="1" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18">
       <c r="A31" s="1" t="s">
         <v>160</v>
       </c>
@@ -18984,8 +19210,14 @@
       <c r="P31" s="1" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="32" spans="1:16">
+      <c r="Q31" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R31" s="1" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18">
       <c r="A32" s="1" t="s">
         <v>164</v>
       </c>
@@ -19030,6 +19262,12 @@
       </c>
       <c r="P32" s="1" t="s">
         <v>1064</v>
+      </c>
+      <c r="Q32" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R32" s="1" t="s">
+        <v>1322</v>
       </c>
     </row>
     <row r="33" spans="1:16">
@@ -20536,7 +20774,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="65" spans="1:16">
+    <row r="65" spans="1:18">
       <c r="A65" s="1" t="s">
         <v>288</v>
       </c>
@@ -20585,8 +20823,14 @@
       <c r="P65" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="66" spans="1:16">
+      <c r="Q65" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R65" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18">
       <c r="A66" s="1" t="s">
         <v>291</v>
       </c>
@@ -20635,8 +20879,14 @@
       <c r="P66" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="67" spans="1:16">
+      <c r="Q66" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R66" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18">
       <c r="A67" s="1" t="s">
         <v>294</v>
       </c>
@@ -20685,8 +20935,14 @@
       <c r="P67" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="68" spans="1:16">
+      <c r="Q67" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R67" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18">
       <c r="A68" s="1" t="s">
         <v>297</v>
       </c>
@@ -20735,8 +20991,14 @@
       <c r="P68" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="69" spans="1:16">
+      <c r="Q68" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R68" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18">
       <c r="A69" s="1" t="s">
         <v>300</v>
       </c>
@@ -20785,8 +21047,14 @@
       <c r="P69" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="70" spans="1:16">
+      <c r="Q69" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R69" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18">
       <c r="A70" s="1" t="s">
         <v>303</v>
       </c>
@@ -20835,8 +21103,14 @@
       <c r="P70" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="71" spans="1:16">
+      <c r="Q70" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R70" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18">
       <c r="A71" s="1" t="s">
         <v>306</v>
       </c>
@@ -20885,8 +21159,14 @@
       <c r="P71" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="72" spans="1:16">
+      <c r="Q71" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R71" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18">
       <c r="A72" s="1" t="s">
         <v>309</v>
       </c>
@@ -20935,8 +21215,14 @@
       <c r="P72" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="73" spans="1:16">
+      <c r="Q72" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R72" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18">
       <c r="A73" s="1" t="s">
         <v>312</v>
       </c>
@@ -20985,8 +21271,14 @@
       <c r="P73" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="74" spans="1:16">
+      <c r="Q73" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R73" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18">
       <c r="A74" s="1" t="s">
         <v>315</v>
       </c>
@@ -21035,8 +21327,14 @@
       <c r="P74" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="75" spans="1:16">
+      <c r="Q74" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R74" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18">
       <c r="A75" s="1" t="s">
         <v>318</v>
       </c>
@@ -21085,8 +21383,14 @@
       <c r="P75" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="76" spans="1:16">
+      <c r="Q75" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R75" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18">
       <c r="A76" s="1" t="s">
         <v>322</v>
       </c>
@@ -21135,8 +21439,14 @@
       <c r="P76" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="77" spans="1:16">
+      <c r="Q76" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R76" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18">
       <c r="A77" s="1" t="s">
         <v>326</v>
       </c>
@@ -21185,8 +21495,14 @@
       <c r="P77" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="78" spans="1:16">
+      <c r="Q77" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R77" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18">
       <c r="A78" s="1" t="s">
         <v>330</v>
       </c>
@@ -21235,8 +21551,14 @@
       <c r="P78" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="79" spans="1:16">
+      <c r="Q78" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R78" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18">
       <c r="A79" s="1" t="s">
         <v>334</v>
       </c>
@@ -21285,8 +21607,14 @@
       <c r="P79" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="80" spans="1:16">
+      <c r="Q79" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R79" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18">
       <c r="A80" s="1" t="s">
         <v>338</v>
       </c>
@@ -21335,8 +21663,14 @@
       <c r="P80" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="81" spans="1:16">
+      <c r="Q80" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R80" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18">
       <c r="A81" s="1" t="s">
         <v>342</v>
       </c>
@@ -21385,8 +21719,14 @@
       <c r="P81" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="82" spans="1:16">
+      <c r="Q81" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R81" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18">
       <c r="A82" s="1" t="s">
         <v>345</v>
       </c>
@@ -21435,8 +21775,14 @@
       <c r="P82" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="83" spans="1:16">
+      <c r="Q82" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R82" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18">
       <c r="A83" s="1" t="s">
         <v>348</v>
       </c>
@@ -21485,8 +21831,14 @@
       <c r="P83" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="84" spans="1:16">
+      <c r="Q83" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R83" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18">
       <c r="A84" s="1" t="s">
         <v>351</v>
       </c>
@@ -21535,8 +21887,14 @@
       <c r="P84" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="85" spans="1:16">
+      <c r="Q84" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R84" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18">
       <c r="A85" s="1" t="s">
         <v>354</v>
       </c>
@@ -21585,8 +21943,14 @@
       <c r="P85" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="86" spans="1:16">
+      <c r="Q85" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R85" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18">
       <c r="A86" s="1" t="s">
         <v>357</v>
       </c>
@@ -21635,8 +21999,14 @@
       <c r="P86" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="87" spans="1:16">
+      <c r="Q86" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R86" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18">
       <c r="A87" s="1" t="s">
         <v>360</v>
       </c>
@@ -21685,8 +22055,14 @@
       <c r="P87" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="88" spans="1:16">
+      <c r="Q87" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R87" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18">
       <c r="A88" s="1" t="s">
         <v>363</v>
       </c>
@@ -21735,8 +22111,14 @@
       <c r="P88" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="89" spans="1:16">
+      <c r="Q88" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R88" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18">
       <c r="A89" s="1" t="s">
         <v>366</v>
       </c>
@@ -21785,8 +22167,14 @@
       <c r="P89" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="90" spans="1:16">
+      <c r="Q89" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R89" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18">
       <c r="A90" s="1" t="s">
         <v>369</v>
       </c>
@@ -21835,8 +22223,14 @@
       <c r="P90" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="91" spans="1:16">
+      <c r="Q90" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R90" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18">
       <c r="A91" s="1" t="s">
         <v>372</v>
       </c>
@@ -21885,8 +22279,14 @@
       <c r="P91" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="92" spans="1:16">
+      <c r="Q91" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R91" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18">
       <c r="A92" s="1" t="s">
         <v>376</v>
       </c>
@@ -21935,8 +22335,14 @@
       <c r="P92" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="93" spans="1:16">
+      <c r="Q92" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R92" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18">
       <c r="A93" s="1" t="s">
         <v>380</v>
       </c>
@@ -21985,8 +22391,14 @@
       <c r="P93" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="94" spans="1:16">
+      <c r="Q93" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R93" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18">
       <c r="A94" s="1" t="s">
         <v>384</v>
       </c>
@@ -22035,8 +22447,14 @@
       <c r="P94" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="95" spans="1:16">
+      <c r="Q94" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R94" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18">
       <c r="A95" s="1" t="s">
         <v>388</v>
       </c>
@@ -22085,8 +22503,14 @@
       <c r="P95" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="96" spans="1:16">
+      <c r="Q95" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R95" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18">
       <c r="A96" s="1" t="s">
         <v>392</v>
       </c>
@@ -22135,8 +22559,14 @@
       <c r="P96" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="97" spans="1:16">
+      <c r="Q96" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R96" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18">
       <c r="A97" s="1" t="s">
         <v>396</v>
       </c>
@@ -22185,8 +22615,14 @@
       <c r="P97" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="98" spans="1:16">
+      <c r="Q97" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R97" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18">
       <c r="A98" s="1" t="s">
         <v>399</v>
       </c>
@@ -22235,8 +22671,14 @@
       <c r="P98" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="99" spans="1:16">
+      <c r="Q98" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R98" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="99" spans="1:18">
       <c r="A99" s="1" t="s">
         <v>402</v>
       </c>
@@ -22285,8 +22727,14 @@
       <c r="P99" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="100" spans="1:16">
+      <c r="Q99" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R99" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18">
       <c r="A100" s="1" t="s">
         <v>405</v>
       </c>
@@ -22335,8 +22783,14 @@
       <c r="P100" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="101" spans="1:16">
+      <c r="Q100" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R100" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18">
       <c r="A101" s="1" t="s">
         <v>408</v>
       </c>
@@ -22385,8 +22839,14 @@
       <c r="P101" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="102" spans="1:16">
+      <c r="Q101" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R101" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18">
       <c r="A102" s="1" t="s">
         <v>411</v>
       </c>
@@ -22435,8 +22895,14 @@
       <c r="P102" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="103" spans="1:16">
+      <c r="Q102" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R102" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="103" spans="1:18">
       <c r="A103" s="1" t="s">
         <v>414</v>
       </c>
@@ -22485,8 +22951,14 @@
       <c r="P103" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="104" spans="1:16">
+      <c r="Q103" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R103" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="104" spans="1:18">
       <c r="A104" s="1" t="s">
         <v>417</v>
       </c>
@@ -22535,8 +23007,14 @@
       <c r="P104" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="105" spans="1:16">
+      <c r="Q104" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R104" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18">
       <c r="A105" s="1" t="s">
         <v>420</v>
       </c>
@@ -22585,8 +23063,14 @@
       <c r="P105" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="106" spans="1:16">
+      <c r="Q105" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R105" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18">
       <c r="A106" s="1" t="s">
         <v>423</v>
       </c>
@@ -22635,8 +23119,14 @@
       <c r="P106" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="107" spans="1:16">
+      <c r="Q106" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R106" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="107" spans="1:18">
       <c r="A107" s="1" t="s">
         <v>426</v>
       </c>
@@ -22685,8 +23175,14 @@
       <c r="P107" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="108" spans="1:16">
+      <c r="Q107" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R107" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="108" spans="1:18">
       <c r="A108" s="1" t="s">
         <v>430</v>
       </c>
@@ -22735,8 +23231,14 @@
       <c r="P108" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="109" spans="1:16">
+      <c r="Q108" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R108" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="109" spans="1:18">
       <c r="A109" s="1" t="s">
         <v>434</v>
       </c>
@@ -22785,8 +23287,14 @@
       <c r="P109" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="110" spans="1:16">
+      <c r="Q109" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R109" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="110" spans="1:18">
       <c r="A110" s="1" t="s">
         <v>438</v>
       </c>
@@ -22835,8 +23343,14 @@
       <c r="P110" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="111" spans="1:16">
+      <c r="Q110" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R110" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="111" spans="1:18">
       <c r="A111" s="1" t="s">
         <v>442</v>
       </c>
@@ -22885,8 +23399,14 @@
       <c r="P111" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="112" spans="1:16">
+      <c r="Q111" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R111" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="112" spans="1:18">
       <c r="A112" s="1" t="s">
         <v>446</v>
       </c>
@@ -22935,8 +23455,14 @@
       <c r="P112" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="113" spans="1:16">
+      <c r="Q112" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R112" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="113" spans="1:18">
       <c r="A113" s="1" t="s">
         <v>450</v>
       </c>
@@ -22985,8 +23511,14 @@
       <c r="P113" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="114" spans="1:16">
+      <c r="Q113" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R113" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="114" spans="1:18">
       <c r="A114" s="1" t="s">
         <v>453</v>
       </c>
@@ -23035,8 +23567,14 @@
       <c r="P114" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="115" spans="1:16">
+      <c r="Q114" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R114" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="115" spans="1:18">
       <c r="A115" s="1" t="s">
         <v>456</v>
       </c>
@@ -23085,8 +23623,14 @@
       <c r="P115" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="116" spans="1:16">
+      <c r="Q115" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R115" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="116" spans="1:18">
       <c r="A116" s="1" t="s">
         <v>459</v>
       </c>
@@ -23135,8 +23679,14 @@
       <c r="P116" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="117" spans="1:16">
+      <c r="Q116" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R116" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="117" spans="1:18">
       <c r="A117" s="1" t="s">
         <v>462</v>
       </c>
@@ -23185,8 +23735,14 @@
       <c r="P117" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="118" spans="1:16">
+      <c r="Q117" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R117" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="118" spans="1:18">
       <c r="A118" s="1" t="s">
         <v>465</v>
       </c>
@@ -23235,8 +23791,14 @@
       <c r="P118" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="119" spans="1:16">
+      <c r="Q118" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R118" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="119" spans="1:18">
       <c r="A119" s="1" t="s">
         <v>468</v>
       </c>
@@ -23285,8 +23847,14 @@
       <c r="P119" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="120" spans="1:16">
+      <c r="Q119" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R119" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="120" spans="1:18">
       <c r="A120" s="1" t="s">
         <v>472</v>
       </c>
@@ -23335,8 +23903,14 @@
       <c r="P120" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="121" spans="1:16">
+      <c r="Q120" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R120" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="121" spans="1:18">
       <c r="A121" s="1" t="s">
         <v>475</v>
       </c>
@@ -23385,8 +23959,14 @@
       <c r="P121" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="122" spans="1:16">
+      <c r="Q121" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R121" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="122" spans="1:18">
       <c r="A122" s="1" t="s">
         <v>478</v>
       </c>
@@ -23435,8 +24015,14 @@
       <c r="P122" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="123" spans="1:16">
+      <c r="Q122" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R122" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="123" spans="1:18">
       <c r="A123" s="1" t="s">
         <v>481</v>
       </c>
@@ -23485,8 +24071,14 @@
       <c r="P123" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="124" spans="1:16">
+      <c r="Q123" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R123" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="124" spans="1:18">
       <c r="A124" s="1" t="s">
         <v>485</v>
       </c>
@@ -23535,8 +24127,14 @@
       <c r="P124" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="125" spans="1:16">
+      <c r="Q124" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R124" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="125" spans="1:18">
       <c r="A125" s="1" t="s">
         <v>489</v>
       </c>
@@ -23585,8 +24183,14 @@
       <c r="P125" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="126" spans="1:16">
+      <c r="Q125" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R125" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="126" spans="1:18">
       <c r="A126" s="1" t="s">
         <v>493</v>
       </c>
@@ -23635,8 +24239,14 @@
       <c r="P126" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="127" spans="1:16">
+      <c r="Q126" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R126" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="127" spans="1:18">
       <c r="A127" s="1" t="s">
         <v>497</v>
       </c>
@@ -23685,8 +24295,14 @@
       <c r="P127" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="128" spans="1:16">
+      <c r="Q127" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R127" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="128" spans="1:18">
       <c r="A128" s="1" t="s">
         <v>501</v>
       </c>
@@ -23735,8 +24351,14 @@
       <c r="P128" s="1" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="129" spans="1:16">
+      <c r="Q128" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R128" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="129" spans="1:18">
       <c r="A129" s="1" t="s">
         <v>505</v>
       </c>
@@ -23785,8 +24407,14 @@
       <c r="P129" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="130" spans="1:16">
+      <c r="Q129" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R129" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="130" spans="1:18">
       <c r="A130" s="1" t="s">
         <v>508</v>
       </c>
@@ -23835,8 +24463,14 @@
       <c r="P130" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="131" spans="1:16">
+      <c r="Q130" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R130" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="131" spans="1:18">
       <c r="A131" s="1" t="s">
         <v>511</v>
       </c>
@@ -23885,8 +24519,14 @@
       <c r="P131" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="132" spans="1:16">
+      <c r="Q131" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R131" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="132" spans="1:18">
       <c r="A132" s="1" t="s">
         <v>514</v>
       </c>
@@ -23935,8 +24575,14 @@
       <c r="P132" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="133" spans="1:16">
+      <c r="Q132" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R132" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="133" spans="1:18">
       <c r="A133" s="1" t="s">
         <v>517</v>
       </c>
@@ -23985,8 +24631,14 @@
       <c r="P133" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="134" spans="1:16">
+      <c r="Q133" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R133" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="134" spans="1:18">
       <c r="A134" s="1" t="s">
         <v>520</v>
       </c>
@@ -24035,8 +24687,14 @@
       <c r="P134" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="135" spans="1:16">
+      <c r="Q134" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R134" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="135" spans="1:18">
       <c r="A135" s="1" t="s">
         <v>523</v>
       </c>
@@ -24085,8 +24743,14 @@
       <c r="P135" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="136" spans="1:16">
+      <c r="Q135" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R135" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="136" spans="1:18">
       <c r="A136" s="1" t="s">
         <v>526</v>
       </c>
@@ -24135,8 +24799,14 @@
       <c r="P136" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="137" spans="1:16">
+      <c r="Q136" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R136" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="137" spans="1:18">
       <c r="A137" s="1" t="s">
         <v>529</v>
       </c>
@@ -24185,8 +24855,14 @@
       <c r="P137" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="138" spans="1:16">
+      <c r="Q137" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R137" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="138" spans="1:18">
       <c r="A138" s="1" t="s">
         <v>534</v>
       </c>
@@ -24235,8 +24911,14 @@
       <c r="P138" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="139" spans="1:16">
+      <c r="Q138" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R138" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="139" spans="1:18">
       <c r="A139" s="1" t="s">
         <v>537</v>
       </c>
@@ -24285,8 +24967,14 @@
       <c r="P139" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="140" spans="1:16">
+      <c r="Q139" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R139" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="140" spans="1:18">
       <c r="A140" s="1" t="s">
         <v>541</v>
       </c>
@@ -24335,8 +25023,14 @@
       <c r="P140" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="141" spans="1:16">
+      <c r="Q140" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R140" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="141" spans="1:18">
       <c r="A141" s="1" t="s">
         <v>545</v>
       </c>
@@ -24385,8 +25079,14 @@
       <c r="P141" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="142" spans="1:16">
+      <c r="Q141" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R141" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="142" spans="1:18">
       <c r="A142" s="1" t="s">
         <v>549</v>
       </c>
@@ -24435,8 +25135,14 @@
       <c r="P142" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="143" spans="1:16">
+      <c r="Q142" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R142" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="143" spans="1:18">
       <c r="A143" s="1" t="s">
         <v>553</v>
       </c>
@@ -24485,8 +25191,14 @@
       <c r="P143" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="144" spans="1:16">
+      <c r="Q143" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R143" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="144" spans="1:18">
       <c r="A144" s="1" t="s">
         <v>557</v>
       </c>
@@ -24535,8 +25247,14 @@
       <c r="P144" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="145" spans="1:16">
+      <c r="Q144" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R144" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="145" spans="1:18">
       <c r="A145" s="1" t="s">
         <v>561</v>
       </c>
@@ -24585,8 +25303,14 @@
       <c r="P145" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="146" spans="1:16">
+      <c r="Q145" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R145" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="146" spans="1:18">
       <c r="A146" s="1" t="s">
         <v>566</v>
       </c>
@@ -24635,8 +25359,14 @@
       <c r="P146" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="147" spans="1:16">
+      <c r="Q146" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R146" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="147" spans="1:18">
       <c r="A147" s="1" t="s">
         <v>569</v>
       </c>
@@ -24685,8 +25415,14 @@
       <c r="P147" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="148" spans="1:16">
+      <c r="Q147" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R147" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="148" spans="1:18">
       <c r="A148" s="1" t="s">
         <v>572</v>
       </c>
@@ -24735,8 +25471,14 @@
       <c r="P148" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="149" spans="1:16">
+      <c r="Q148" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R148" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="149" spans="1:18">
       <c r="A149" s="1" t="s">
         <v>575</v>
       </c>
@@ -24785,8 +25527,14 @@
       <c r="P149" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="150" spans="1:16">
+      <c r="Q149" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R149" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="150" spans="1:18">
       <c r="A150" s="1" t="s">
         <v>578</v>
       </c>
@@ -24835,8 +25583,14 @@
       <c r="P150" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="151" spans="1:16">
+      <c r="Q150" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R150" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="151" spans="1:18">
       <c r="A151" s="1" t="s">
         <v>581</v>
       </c>
@@ -24885,8 +25639,14 @@
       <c r="P151" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="152" spans="1:16">
+      <c r="Q151" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R151" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="152" spans="1:18">
       <c r="A152" s="1" t="s">
         <v>584</v>
       </c>
@@ -24935,8 +25695,14 @@
       <c r="P152" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="153" spans="1:16">
+      <c r="Q152" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R152" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="153" spans="1:18">
       <c r="A153" s="1" t="s">
         <v>587</v>
       </c>
@@ -24985,8 +25751,14 @@
       <c r="P153" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="154" spans="1:16">
+      <c r="Q153" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R153" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="154" spans="1:18">
       <c r="A154" s="1" t="s">
         <v>592</v>
       </c>
@@ -25035,8 +25807,14 @@
       <c r="P154" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="155" spans="1:16">
+      <c r="Q154" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R154" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="155" spans="1:18">
       <c r="A155" s="1" t="s">
         <v>595</v>
       </c>
@@ -25085,8 +25863,14 @@
       <c r="P155" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="156" spans="1:16">
+      <c r="Q155" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R155" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="156" spans="1:18">
       <c r="A156" s="1" t="s">
         <v>599</v>
       </c>
@@ -25135,8 +25919,14 @@
       <c r="P156" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="157" spans="1:16">
+      <c r="Q156" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R156" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="157" spans="1:18">
       <c r="A157" s="1" t="s">
         <v>603</v>
       </c>
@@ -25185,8 +25975,14 @@
       <c r="P157" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="158" spans="1:16">
+      <c r="Q157" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R157" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="158" spans="1:18">
       <c r="A158" s="1" t="s">
         <v>607</v>
       </c>
@@ -25235,8 +26031,14 @@
       <c r="P158" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="159" spans="1:16">
+      <c r="Q158" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R158" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="159" spans="1:18">
       <c r="A159" s="1" t="s">
         <v>611</v>
       </c>
@@ -25285,8 +26087,14 @@
       <c r="P159" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="160" spans="1:16">
+      <c r="Q159" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R159" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="160" spans="1:18">
       <c r="A160" s="1" t="s">
         <v>615</v>
       </c>
@@ -25335,8 +26143,14 @@
       <c r="P160" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="161" spans="1:16">
+      <c r="Q160" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R160" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="161" spans="1:18">
       <c r="A161" s="1" t="s">
         <v>619</v>
       </c>
@@ -25385,8 +26199,14 @@
       <c r="P161" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="162" spans="1:16">
+      <c r="Q161" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R161" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="162" spans="1:18">
       <c r="A162" s="1" t="s">
         <v>625</v>
       </c>
@@ -25435,8 +26255,14 @@
       <c r="P162" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="163" spans="1:16">
+      <c r="Q162" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R162" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="163" spans="1:18">
       <c r="A163" s="1" t="s">
         <v>629</v>
       </c>
@@ -25485,8 +26311,14 @@
       <c r="P163" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="164" spans="1:16">
+      <c r="Q163" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R163" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="164" spans="1:18">
       <c r="A164" s="1" t="s">
         <v>633</v>
       </c>
@@ -25535,8 +26367,14 @@
       <c r="P164" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="165" spans="1:16">
+      <c r="Q164" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R164" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="165" spans="1:18">
       <c r="A165" s="1" t="s">
         <v>637</v>
       </c>
@@ -25585,8 +26423,14 @@
       <c r="P165" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="166" spans="1:16">
+      <c r="Q165" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R165" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="166" spans="1:18">
       <c r="A166" s="1" t="s">
         <v>641</v>
       </c>
@@ -25635,8 +26479,14 @@
       <c r="P166" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="167" spans="1:16">
+      <c r="Q166" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R166" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="167" spans="1:18">
       <c r="A167" s="1" t="s">
         <v>645</v>
       </c>
@@ -25685,8 +26535,14 @@
       <c r="P167" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="168" spans="1:16">
+      <c r="Q167" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R167" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="168" spans="1:18">
       <c r="A168" s="1" t="s">
         <v>649</v>
       </c>
@@ -25735,8 +26591,14 @@
       <c r="P168" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="169" spans="1:16">
+      <c r="Q168" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R168" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="169" spans="1:18">
       <c r="A169" s="1" t="s">
         <v>653</v>
       </c>
@@ -25785,8 +26647,14 @@
       <c r="P169" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="170" spans="1:16">
+      <c r="Q169" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R169" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="170" spans="1:18">
       <c r="A170" s="1" t="s">
         <v>659</v>
       </c>
@@ -25835,8 +26703,14 @@
       <c r="P170" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="171" spans="1:16">
+      <c r="Q170" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R170" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="171" spans="1:18">
       <c r="A171" s="1" t="s">
         <v>663</v>
       </c>
@@ -25885,8 +26759,14 @@
       <c r="P171" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="172" spans="1:16">
+      <c r="Q171" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R171" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="172" spans="1:18">
       <c r="A172" s="1" t="s">
         <v>667</v>
       </c>
@@ -25935,8 +26815,14 @@
       <c r="P172" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="173" spans="1:16">
+      <c r="Q172" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R172" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="173" spans="1:18">
       <c r="A173" s="1" t="s">
         <v>671</v>
       </c>
@@ -25985,8 +26871,14 @@
       <c r="P173" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="174" spans="1:16">
+      <c r="Q173" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R173" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="174" spans="1:18">
       <c r="A174" s="1" t="s">
         <v>675</v>
       </c>
@@ -26035,8 +26927,14 @@
       <c r="P174" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="175" spans="1:16">
+      <c r="Q174" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R174" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="175" spans="1:18">
       <c r="A175" s="1" t="s">
         <v>679</v>
       </c>
@@ -26085,8 +26983,14 @@
       <c r="P175" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="176" spans="1:16">
+      <c r="Q175" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R175" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="176" spans="1:18">
       <c r="A176" s="1" t="s">
         <v>683</v>
       </c>
@@ -26135,8 +27039,14 @@
       <c r="P176" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="177" spans="1:16">
+      <c r="Q176" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R176" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="177" spans="1:18">
       <c r="A177" s="1" t="s">
         <v>687</v>
       </c>
@@ -26185,8 +27095,14 @@
       <c r="P177" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="178" spans="1:16">
+      <c r="Q177" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R177" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="178" spans="1:18">
       <c r="A178" s="1" t="s">
         <v>693</v>
       </c>
@@ -26235,8 +27151,14 @@
       <c r="P178" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="179" spans="1:16">
+      <c r="Q178" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R178" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="179" spans="1:18">
       <c r="A179" s="1" t="s">
         <v>697</v>
       </c>
@@ -26285,8 +27207,14 @@
       <c r="P179" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="180" spans="1:16">
+      <c r="Q179" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R179" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="180" spans="1:18">
       <c r="A180" s="1" t="s">
         <v>701</v>
       </c>
@@ -26335,8 +27263,14 @@
       <c r="P180" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="181" spans="1:16">
+      <c r="Q180" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R180" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="181" spans="1:18">
       <c r="A181" s="1" t="s">
         <v>705</v>
       </c>
@@ -26385,8 +27319,14 @@
       <c r="P181" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="182" spans="1:16">
+      <c r="Q181" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R181" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="182" spans="1:18">
       <c r="A182" s="1" t="s">
         <v>709</v>
       </c>
@@ -26435,8 +27375,14 @@
       <c r="P182" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="183" spans="1:16">
+      <c r="Q182" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R182" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="183" spans="1:18">
       <c r="A183" s="1" t="s">
         <v>713</v>
       </c>
@@ -26485,8 +27431,14 @@
       <c r="P183" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="184" spans="1:16">
+      <c r="Q183" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R183" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="184" spans="1:18">
       <c r="A184" s="1" t="s">
         <v>717</v>
       </c>
@@ -26535,8 +27487,14 @@
       <c r="P184" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="185" spans="1:16">
+      <c r="Q184" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R184" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="185" spans="1:18">
       <c r="A185" s="1" t="s">
         <v>721</v>
       </c>
@@ -26585,8 +27543,14 @@
       <c r="P185" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="186" spans="1:16">
+      <c r="Q185" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R185" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="186" spans="1:18">
       <c r="A186" s="1" t="s">
         <v>727</v>
       </c>
@@ -26635,8 +27599,14 @@
       <c r="P186" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="187" spans="1:16">
+      <c r="Q186" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R186" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="187" spans="1:18">
       <c r="A187" s="1" t="s">
         <v>731</v>
       </c>
@@ -26685,8 +27655,14 @@
       <c r="P187" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="188" spans="1:16">
+      <c r="Q187" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R187" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="188" spans="1:18">
       <c r="A188" s="1" t="s">
         <v>735</v>
       </c>
@@ -26735,8 +27711,14 @@
       <c r="P188" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="189" spans="1:16">
+      <c r="Q188" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R188" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="189" spans="1:18">
       <c r="A189" s="1" t="s">
         <v>739</v>
       </c>
@@ -26785,8 +27767,14 @@
       <c r="P189" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="190" spans="1:16">
+      <c r="Q189" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R189" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="190" spans="1:18">
       <c r="A190" s="1" t="s">
         <v>742</v>
       </c>
@@ -26835,8 +27823,14 @@
       <c r="P190" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="191" spans="1:16">
+      <c r="Q190" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R190" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="191" spans="1:18">
       <c r="A191" s="1" t="s">
         <v>746</v>
       </c>
@@ -26885,8 +27879,14 @@
       <c r="P191" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="192" spans="1:16">
+      <c r="Q191" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R191" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="192" spans="1:18">
       <c r="A192" s="1" t="s">
         <v>750</v>
       </c>
@@ -26935,8 +27935,14 @@
       <c r="P192" s="1" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="193" spans="1:16">
+      <c r="Q192" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R192" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="193" spans="1:18">
       <c r="A193" s="1" t="s">
         <v>754</v>
       </c>
@@ -26985,8 +27991,14 @@
       <c r="P193" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="194" spans="1:16">
+      <c r="Q193" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R193" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="194" spans="1:18">
       <c r="A194" s="1" t="s">
         <v>761</v>
       </c>
@@ -27035,8 +28047,14 @@
       <c r="P194" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="195" spans="1:16">
+      <c r="Q194" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R194" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="195" spans="1:18">
       <c r="A195" s="1" t="s">
         <v>767</v>
       </c>
@@ -27085,8 +28103,14 @@
       <c r="P195" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="196" spans="1:16">
+      <c r="Q195" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R195" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="196" spans="1:18">
       <c r="A196" s="1" t="s">
         <v>775</v>
       </c>
@@ -27135,8 +28159,14 @@
       <c r="P196" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="197" spans="1:16">
+      <c r="Q196" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R196" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="197" spans="1:18">
       <c r="A197" s="1" t="s">
         <v>779</v>
       </c>
@@ -27185,8 +28215,14 @@
       <c r="P197" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="198" spans="1:16">
+      <c r="Q197" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R197" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="198" spans="1:18">
       <c r="A198" s="1" t="s">
         <v>786</v>
       </c>
@@ -27235,8 +28271,14 @@
       <c r="P198" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="199" spans="1:16">
+      <c r="Q198" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R198" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="199" spans="1:18">
       <c r="A199" s="1" t="s">
         <v>792</v>
       </c>
@@ -27285,8 +28327,14 @@
       <c r="P199" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="200" spans="1:16">
+      <c r="Q199" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R199" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="200" spans="1:18">
       <c r="A200" s="1" t="s">
         <v>796</v>
       </c>
@@ -27335,8 +28383,14 @@
       <c r="P200" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="201" spans="1:16">
+      <c r="Q200" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R200" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="201" spans="1:18">
       <c r="A201" s="1" t="s">
         <v>803</v>
       </c>
@@ -27385,8 +28439,14 @@
       <c r="P201" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="202" spans="1:16">
+      <c r="Q201" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R201" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="202" spans="1:18">
       <c r="A202" s="1" t="s">
         <v>807</v>
       </c>
@@ -27435,8 +28495,14 @@
       <c r="P202" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="203" spans="1:16">
+      <c r="Q202" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R202" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="203" spans="1:18">
       <c r="A203" s="1" t="s">
         <v>810</v>
       </c>
@@ -27485,8 +28551,14 @@
       <c r="P203" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="204" spans="1:16">
+      <c r="Q203" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R203" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="204" spans="1:18">
       <c r="A204" s="1" t="s">
         <v>814</v>
       </c>
@@ -27535,8 +28607,14 @@
       <c r="P204" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="205" spans="1:16">
+      <c r="Q204" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R204" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="205" spans="1:18">
       <c r="A205" s="1" t="s">
         <v>819</v>
       </c>
@@ -27585,8 +28663,14 @@
       <c r="P205" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="206" spans="1:16">
+      <c r="Q205" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R205" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="206" spans="1:18">
       <c r="A206" s="1" t="s">
         <v>823</v>
       </c>
@@ -27635,8 +28719,14 @@
       <c r="P206" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="207" spans="1:16">
+      <c r="Q206" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R206" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="207" spans="1:18">
       <c r="A207" s="1" t="s">
         <v>827</v>
       </c>
@@ -27685,8 +28775,14 @@
       <c r="P207" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="208" spans="1:16">
+      <c r="Q207" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R207" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="208" spans="1:18">
       <c r="A208" s="1" t="s">
         <v>831</v>
       </c>
@@ -27735,8 +28831,14 @@
       <c r="P208" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="209" spans="1:16">
+      <c r="Q208" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R208" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="209" spans="1:18">
       <c r="A209" s="1" t="s">
         <v>836</v>
       </c>
@@ -27785,8 +28887,14 @@
       <c r="P209" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="210" spans="1:16">
+      <c r="Q209" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R209" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="210" spans="1:18">
       <c r="A210" s="1" t="s">
         <v>840</v>
       </c>
@@ -27835,8 +28943,14 @@
       <c r="P210" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="211" spans="1:16">
+      <c r="Q210" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R210" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="211" spans="1:18">
       <c r="A211" s="1" t="s">
         <v>844</v>
       </c>
@@ -27885,8 +28999,14 @@
       <c r="P211" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="212" spans="1:16">
+      <c r="Q211" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R211" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="212" spans="1:18">
       <c r="A212" s="1" t="s">
         <v>848</v>
       </c>
@@ -27935,8 +29055,14 @@
       <c r="P212" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="213" spans="1:16">
+      <c r="Q212" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R212" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="213" spans="1:18">
       <c r="A213" s="1" t="s">
         <v>852</v>
       </c>
@@ -27985,8 +29111,14 @@
       <c r="P213" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="214" spans="1:16">
+      <c r="Q213" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R213" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="214" spans="1:18">
       <c r="A214" s="1" t="s">
         <v>856</v>
       </c>
@@ -28035,8 +29167,14 @@
       <c r="P214" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="215" spans="1:16">
+      <c r="Q214" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R214" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="215" spans="1:18">
       <c r="A215" s="1" t="s">
         <v>860</v>
       </c>
@@ -28085,8 +29223,14 @@
       <c r="P215" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="216" spans="1:16">
+      <c r="Q215" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R215" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="216" spans="1:18">
       <c r="A216" s="1" t="s">
         <v>864</v>
       </c>
@@ -28135,8 +29279,14 @@
       <c r="P216" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="217" spans="1:16">
+      <c r="Q216" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R216" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="217" spans="1:18">
       <c r="A217" s="1" t="s">
         <v>869</v>
       </c>
@@ -28185,8 +29335,14 @@
       <c r="P217" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="218" spans="1:16">
+      <c r="Q217" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R217" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="218" spans="1:18">
       <c r="A218" s="1" t="s">
         <v>873</v>
       </c>
@@ -28235,8 +29391,14 @@
       <c r="P218" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="219" spans="1:16">
+      <c r="Q218" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R218" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="219" spans="1:18">
       <c r="A219" s="1" t="s">
         <v>878</v>
       </c>
@@ -28285,8 +29447,14 @@
       <c r="P219" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="220" spans="1:16">
+      <c r="Q219" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R219" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="220" spans="1:18">
       <c r="A220" s="1" t="s">
         <v>882</v>
       </c>
@@ -28335,8 +29503,14 @@
       <c r="P220" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="221" spans="1:16">
+      <c r="Q220" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R220" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="221" spans="1:18">
       <c r="A221" s="1" t="s">
         <v>885</v>
       </c>
@@ -28385,8 +29559,14 @@
       <c r="P221" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="222" spans="1:16">
+      <c r="Q221" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R221" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="222" spans="1:18">
       <c r="A222" s="1" t="s">
         <v>889</v>
       </c>
@@ -28435,8 +29615,14 @@
       <c r="P222" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="223" spans="1:16">
+      <c r="Q222" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R222" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="223" spans="1:18">
       <c r="A223" s="1" t="s">
         <v>892</v>
       </c>
@@ -28485,8 +29671,14 @@
       <c r="P223" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="224" spans="1:16">
+      <c r="Q223" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R223" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="224" spans="1:18">
       <c r="A224" s="1" t="s">
         <v>895</v>
       </c>
@@ -28535,8 +29727,14 @@
       <c r="P224" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="225" spans="1:16">
+      <c r="Q224" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R224" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="225" spans="1:18">
       <c r="A225" s="1" t="s">
         <v>900</v>
       </c>
@@ -28585,8 +29783,14 @@
       <c r="P225" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="226" spans="1:16">
+      <c r="Q225" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R225" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="226" spans="1:18">
       <c r="A226" s="1" t="s">
         <v>907</v>
       </c>
@@ -28635,8 +29839,14 @@
       <c r="P226" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="227" spans="1:16">
+      <c r="Q226" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R226" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="227" spans="1:18">
       <c r="A227" s="1" t="s">
         <v>911</v>
       </c>
@@ -28685,8 +29895,14 @@
       <c r="P227" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="228" spans="1:16">
+      <c r="Q227" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R227" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="228" spans="1:18">
       <c r="A228" s="1" t="s">
         <v>916</v>
       </c>
@@ -28735,8 +29951,14 @@
       <c r="P228" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="229" spans="1:16">
+      <c r="Q228" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R228" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="229" spans="1:18">
       <c r="A229" s="1" t="s">
         <v>919</v>
       </c>
@@ -28785,8 +30007,14 @@
       <c r="P229" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="230" spans="1:16">
+      <c r="Q229" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R229" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="230" spans="1:18">
       <c r="A230" s="1" t="s">
         <v>922</v>
       </c>
@@ -28835,8 +30063,14 @@
       <c r="P230" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="231" spans="1:16">
+      <c r="Q230" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R230" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="231" spans="1:18">
       <c r="A231" s="1" t="s">
         <v>926</v>
       </c>
@@ -28885,8 +30119,14 @@
       <c r="P231" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="232" spans="1:16">
+      <c r="Q231" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R231" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="232" spans="1:18">
       <c r="A232" s="1" t="s">
         <v>930</v>
       </c>
@@ -28935,8 +30175,14 @@
       <c r="P232" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="233" spans="1:16">
+      <c r="Q232" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R232" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="233" spans="1:18">
       <c r="A233" s="1" t="s">
         <v>935</v>
       </c>
@@ -28985,8 +30231,14 @@
       <c r="P233" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="234" spans="1:16">
+      <c r="Q233" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R233" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="234" spans="1:18">
       <c r="A234" s="1" t="s">
         <v>939</v>
       </c>
@@ -29035,8 +30287,14 @@
       <c r="P234" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="235" spans="1:16">
+      <c r="Q234" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R234" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="235" spans="1:18">
       <c r="A235" s="1" t="s">
         <v>943</v>
       </c>
@@ -29085,8 +30343,14 @@
       <c r="P235" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="236" spans="1:16">
+      <c r="Q235" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R235" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="236" spans="1:18">
       <c r="A236" s="1" t="s">
         <v>947</v>
       </c>
@@ -29135,8 +30399,14 @@
       <c r="P236" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="237" spans="1:16">
+      <c r="Q236" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R236" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="237" spans="1:18">
       <c r="A237" s="1" t="s">
         <v>950</v>
       </c>
@@ -29185,8 +30455,14 @@
       <c r="P237" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="238" spans="1:16">
+      <c r="Q237" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R237" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="238" spans="1:18">
       <c r="A238" s="1" t="s">
         <v>953</v>
       </c>
@@ -29235,8 +30511,14 @@
       <c r="P238" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="239" spans="1:16">
+      <c r="Q238" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R238" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="239" spans="1:18">
       <c r="A239" s="1" t="s">
         <v>956</v>
       </c>
@@ -29285,8 +30567,14 @@
       <c r="P239" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="240" spans="1:16">
+      <c r="Q239" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R239" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="240" spans="1:18">
       <c r="A240" s="1" t="s">
         <v>960</v>
       </c>
@@ -29335,8 +30623,14 @@
       <c r="P240" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="241" spans="1:16">
+      <c r="Q240" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R240" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="241" spans="1:18">
       <c r="A241" s="1" t="s">
         <v>965</v>
       </c>
@@ -29385,8 +30679,14 @@
       <c r="P241" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="242" spans="1:16">
+      <c r="Q241" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R241" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="242" spans="1:18">
       <c r="A242" s="1" t="s">
         <v>969</v>
       </c>
@@ -29435,8 +30735,14 @@
       <c r="P242" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="243" spans="1:16">
+      <c r="Q242" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R242" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="243" spans="1:18">
       <c r="A243" s="1" t="s">
         <v>974</v>
       </c>
@@ -29485,8 +30791,14 @@
       <c r="P243" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="244" spans="1:16">
+      <c r="Q243" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R243" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="244" spans="1:18">
       <c r="A244" s="1" t="s">
         <v>978</v>
       </c>
@@ -29535,8 +30847,14 @@
       <c r="P244" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="245" spans="1:16">
+      <c r="Q244" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R244" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="245" spans="1:18">
       <c r="A245" s="1" t="s">
         <v>983</v>
       </c>
@@ -29585,8 +30903,14 @@
       <c r="P245" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="246" spans="1:16">
+      <c r="Q245" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R245" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="246" spans="1:18">
       <c r="A246" s="1" t="s">
         <v>986</v>
       </c>
@@ -29635,8 +30959,14 @@
       <c r="P246" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="247" spans="1:16">
+      <c r="Q246" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R246" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="247" spans="1:18">
       <c r="A247" s="1" t="s">
         <v>990</v>
       </c>
@@ -29685,8 +31015,14 @@
       <c r="P247" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="248" spans="1:16">
+      <c r="Q247" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R247" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="248" spans="1:18">
       <c r="A248" s="1" t="s">
         <v>994</v>
       </c>
@@ -29735,8 +31071,14 @@
       <c r="P248" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="249" spans="1:16">
+      <c r="Q248" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R248" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="249" spans="1:18">
       <c r="A249" s="1" t="s">
         <v>999</v>
       </c>
@@ -29785,8 +31127,14 @@
       <c r="P249" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="250" spans="1:16">
+      <c r="Q249" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R249" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="250" spans="1:18">
       <c r="A250" s="1" t="s">
         <v>1004</v>
       </c>
@@ -29835,8 +31183,14 @@
       <c r="P250" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="251" spans="1:16">
+      <c r="Q250" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R250" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="251" spans="1:18">
       <c r="A251" s="1" t="s">
         <v>1008</v>
       </c>
@@ -29885,8 +31239,14 @@
       <c r="P251" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="252" spans="1:16">
+      <c r="Q251" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R251" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="252" spans="1:18">
       <c r="A252" s="1" t="s">
         <v>1012</v>
       </c>
@@ -29935,8 +31295,14 @@
       <c r="P252" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="253" spans="1:16">
+      <c r="Q252" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R252" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="253" spans="1:18">
       <c r="A253" s="1" t="s">
         <v>1017</v>
       </c>
@@ -29985,8 +31351,14 @@
       <c r="P253" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="254" spans="1:16">
+      <c r="Q253" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R253" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="254" spans="1:18">
       <c r="A254" s="1" t="s">
         <v>1020</v>
       </c>
@@ -30035,8 +31407,14 @@
       <c r="P254" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="255" spans="1:16">
+      <c r="Q254" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R254" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="255" spans="1:18">
       <c r="A255" s="1" t="s">
         <v>1023</v>
       </c>
@@ -30085,8 +31463,14 @@
       <c r="P255" s="1" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="256" spans="1:16">
+      <c r="Q255" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R255" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="256" spans="1:18">
       <c r="A256" s="1" t="s">
         <v>1027</v>
       </c>
@@ -30135,9 +31519,16 @@
       <c r="P256" s="1" t="s">
         <v>1246</v>
       </c>
+      <c r="Q256" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R256" s="1" t="s">
+        <v>1318</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
More additions to the opcode table.
</commit_message>
<xml_diff>
--- a/other/op_codes_implementations.xlsx
+++ b/other/op_codes_implementations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="360" windowWidth="25940" windowHeight="16080" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="980" yWindow="360" windowWidth="25940" windowHeight="16080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Main Codes" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8648" uniqueCount="1323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8662" uniqueCount="1323">
   <si>
     <t>0</t>
   </si>
@@ -4493,8 +4493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R256"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q49" sqref="Q49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4936,6 +4936,12 @@
       <c r="P8" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="Q8" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>1319</v>
+      </c>
     </row>
     <row r="9" spans="1:18">
       <c r="A9" s="1" t="s">
@@ -5042,6 +5048,12 @@
       <c r="P10" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="Q10" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>1313</v>
+      </c>
     </row>
     <row r="11" spans="1:18">
       <c r="A11" s="1" t="s">
@@ -5357,6 +5369,12 @@
       <c r="P16" s="1" t="s">
         <v>104</v>
       </c>
+      <c r="Q16" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>1320</v>
+      </c>
     </row>
     <row r="17" spans="1:18">
       <c r="A17" s="1" t="s">
@@ -5778,6 +5796,12 @@
       <c r="P24" s="1" t="s">
         <v>133</v>
       </c>
+      <c r="Q24" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>1321</v>
+      </c>
     </row>
     <row r="25" spans="1:18">
       <c r="A25" s="1" t="s">
@@ -5875,6 +5899,12 @@
       <c r="P26" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="Q26" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R26" s="1" t="s">
+        <v>1313</v>
+      </c>
     </row>
     <row r="27" spans="1:18">
       <c r="A27" s="1" t="s">
@@ -6190,6 +6220,12 @@
       <c r="P32" s="1" t="s">
         <v>168</v>
       </c>
+      <c r="Q32" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R32" s="1" t="s">
+        <v>1322</v>
+      </c>
     </row>
     <row r="33" spans="1:18">
       <c r="A33" s="1" t="s">
@@ -6710,6 +6746,12 @@
       </c>
       <c r="P42" s="1" t="s">
         <v>74</v>
+      </c>
+      <c r="Q42" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R42" s="1" t="s">
+        <v>1313</v>
       </c>
     </row>
     <row r="43" spans="1:18">
@@ -17550,7 +17592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R26" sqref="R26:R32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
AND, OR, XOR, comlement methods added, tests pass
</commit_message>
<xml_diff>
--- a/other/op_codes_implementations.xlsx
+++ b/other/op_codes_implementations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="360" windowWidth="25940" windowHeight="16080" tabRatio="500"/>
+    <workbookView xWindow="980" yWindow="360" windowWidth="25940" windowHeight="16080" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Main Codes" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8662" uniqueCount="1323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8710" uniqueCount="1326">
   <si>
     <t>0</t>
   </si>
@@ -4042,6 +4042,15 @@
   </si>
   <si>
     <t>rotateRightThroughFlag</t>
+  </si>
+  <si>
+    <t>rotateRightThroughFlag(n.checkBit(7))</t>
+  </si>
+  <si>
+    <t>rotateLeftThroughFlag(false)</t>
+  </si>
+  <si>
+    <t>rotateRightThroughFlag(false)</t>
   </si>
 </sst>
 </file>
@@ -4090,8 +4099,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4125,7 +4148,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4140,6 +4163,13 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4154,6 +4184,13 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4493,7 +4530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R256"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A233" workbookViewId="0">
       <selection activeCell="Q49" sqref="Q49"/>
     </sheetView>
   </sheetViews>
@@ -17592,8 +17629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R256"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R26" sqref="R26:R32"/>
+    <sheetView tabSelected="1" topLeftCell="A225" workbookViewId="0">
+      <selection activeCell="R53" sqref="R53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -17614,6 +17651,7 @@
     <col min="14" max="14" width="3" customWidth="1"/>
     <col min="15" max="15" width="3.33203125" customWidth="1"/>
     <col min="16" max="16" width="36.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -19312,7 +19350,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:18">
       <c r="A33" s="1" t="s">
         <v>169</v>
       </c>
@@ -19358,8 +19396,14 @@
       <c r="P33" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="34" spans="1:16">
+      <c r="Q33" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R33" s="1" t="s">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18">
       <c r="A34" s="1" t="s">
         <v>174</v>
       </c>
@@ -19405,8 +19449,14 @@
       <c r="P34" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="35" spans="1:16">
+      <c r="Q34" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R34" s="1" t="s">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18">
       <c r="A35" s="1" t="s">
         <v>177</v>
       </c>
@@ -19452,8 +19502,14 @@
       <c r="P35" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="36" spans="1:16">
+      <c r="Q35" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R35" s="1" t="s">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18">
       <c r="A36" s="1" t="s">
         <v>181</v>
       </c>
@@ -19499,8 +19555,14 @@
       <c r="P36" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="37" spans="1:16">
+      <c r="Q36" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R36" s="1" t="s">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18">
       <c r="A37" s="1" t="s">
         <v>184</v>
       </c>
@@ -19546,8 +19608,14 @@
       <c r="P37" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="38" spans="1:16">
+      <c r="Q37" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R37" s="1" t="s">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18">
       <c r="A38" s="1" t="s">
         <v>187</v>
       </c>
@@ -19593,8 +19661,14 @@
       <c r="P38" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="39" spans="1:16">
+      <c r="Q38" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R38" s="1" t="s">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18">
       <c r="A39" s="1" t="s">
         <v>190</v>
       </c>
@@ -19640,8 +19714,14 @@
       <c r="P39" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="40" spans="1:16">
+      <c r="Q39" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R39" s="1" t="s">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18">
       <c r="A40" s="1" t="s">
         <v>193</v>
       </c>
@@ -19687,8 +19767,14 @@
       <c r="P40" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="41" spans="1:16">
+      <c r="Q40" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R40" s="1" t="s">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18">
       <c r="A41" s="1" t="s">
         <v>197</v>
       </c>
@@ -19734,8 +19820,14 @@
       <c r="P41" s="1" t="s">
         <v>1084</v>
       </c>
-    </row>
-    <row r="42" spans="1:16">
+      <c r="Q41" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R41" s="1" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18">
       <c r="A42" s="1" t="s">
         <v>200</v>
       </c>
@@ -19781,8 +19873,14 @@
       <c r="P42" s="1" t="s">
         <v>1084</v>
       </c>
-    </row>
-    <row r="43" spans="1:16">
+      <c r="Q42" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R42" s="1" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18">
       <c r="A43" s="1" t="s">
         <v>203</v>
       </c>
@@ -19828,8 +19926,14 @@
       <c r="P43" s="1" t="s">
         <v>1084</v>
       </c>
-    </row>
-    <row r="44" spans="1:16">
+      <c r="Q43" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R43" s="1" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18">
       <c r="A44" s="1" t="s">
         <v>207</v>
       </c>
@@ -19875,8 +19979,14 @@
       <c r="P44" s="1" t="s">
         <v>1084</v>
       </c>
-    </row>
-    <row r="45" spans="1:16">
+      <c r="Q44" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R44" s="1" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18">
       <c r="A45" s="1" t="s">
         <v>211</v>
       </c>
@@ -19922,8 +20032,14 @@
       <c r="P45" s="1" t="s">
         <v>1084</v>
       </c>
-    </row>
-    <row r="46" spans="1:16">
+      <c r="Q45" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R45" s="1" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18">
       <c r="A46" s="1" t="s">
         <v>216</v>
       </c>
@@ -19969,8 +20085,14 @@
       <c r="P46" s="1" t="s">
         <v>1084</v>
       </c>
-    </row>
-    <row r="47" spans="1:16">
+      <c r="Q46" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R46" s="1" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18">
       <c r="A47" s="1" t="s">
         <v>220</v>
       </c>
@@ -20016,8 +20138,14 @@
       <c r="P47" s="1" t="s">
         <v>1084</v>
       </c>
-    </row>
-    <row r="48" spans="1:16">
+      <c r="Q47" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R47" s="1" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18">
       <c r="A48" s="1" t="s">
         <v>224</v>
       </c>
@@ -20063,8 +20191,14 @@
       <c r="P48" s="1" t="s">
         <v>1084</v>
       </c>
-    </row>
-    <row r="49" spans="1:16">
+      <c r="Q48" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R48" s="1" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18">
       <c r="A49" s="1" t="s">
         <v>229</v>
       </c>
@@ -20111,7 +20245,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="50" spans="1:16">
+    <row r="50" spans="1:18">
       <c r="A50" s="1" t="s">
         <v>233</v>
       </c>
@@ -20158,7 +20292,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="51" spans="1:16">
+    <row r="51" spans="1:18">
       <c r="A51" s="1" t="s">
         <v>236</v>
       </c>
@@ -20205,7 +20339,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="52" spans="1:16">
+    <row r="52" spans="1:18">
       <c r="A52" s="1" t="s">
         <v>240</v>
       </c>
@@ -20252,7 +20386,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="53" spans="1:16">
+    <row r="53" spans="1:18">
       <c r="A53" s="1" t="s">
         <v>243</v>
       </c>
@@ -20299,7 +20433,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="54" spans="1:16">
+    <row r="54" spans="1:18">
       <c r="A54" s="1" t="s">
         <v>247</v>
       </c>
@@ -20346,7 +20480,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="55" spans="1:16">
+    <row r="55" spans="1:18">
       <c r="A55" s="1" t="s">
         <v>250</v>
       </c>
@@ -20393,7 +20527,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="56" spans="1:16">
+    <row r="56" spans="1:18">
       <c r="A56" s="1" t="s">
         <v>253</v>
       </c>
@@ -20440,7 +20574,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="57" spans="1:16">
+    <row r="57" spans="1:18">
       <c r="A57" s="1" t="s">
         <v>257</v>
       </c>
@@ -20486,8 +20620,14 @@
       <c r="P57" s="1" t="s">
         <v>1104</v>
       </c>
-    </row>
-    <row r="58" spans="1:16">
+      <c r="Q57" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R57" s="1" t="s">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18">
       <c r="A58" s="1" t="s">
         <v>260</v>
       </c>
@@ -20533,8 +20673,14 @@
       <c r="P58" s="1" t="s">
         <v>1104</v>
       </c>
-    </row>
-    <row r="59" spans="1:16">
+      <c r="Q58" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R58" s="1" t="s">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18">
       <c r="A59" s="1" t="s">
         <v>263</v>
       </c>
@@ -20580,8 +20726,14 @@
       <c r="P59" s="1" t="s">
         <v>1104</v>
       </c>
-    </row>
-    <row r="60" spans="1:16">
+      <c r="Q59" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R59" s="1" t="s">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18">
       <c r="A60" s="1" t="s">
         <v>267</v>
       </c>
@@ -20627,8 +20779,14 @@
       <c r="P60" s="1" t="s">
         <v>1104</v>
       </c>
-    </row>
-    <row r="61" spans="1:16">
+      <c r="Q60" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R60" s="1" t="s">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18">
       <c r="A61" s="1" t="s">
         <v>271</v>
       </c>
@@ -20674,8 +20832,14 @@
       <c r="P61" s="1" t="s">
         <v>1104</v>
       </c>
-    </row>
-    <row r="62" spans="1:16">
+      <c r="Q61" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R61" s="1" t="s">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18">
       <c r="A62" s="1" t="s">
         <v>275</v>
       </c>
@@ -20721,8 +20885,14 @@
       <c r="P62" s="1" t="s">
         <v>1104</v>
       </c>
-    </row>
-    <row r="63" spans="1:16">
+      <c r="Q62" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R62" s="1" t="s">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18">
       <c r="A63" s="1" t="s">
         <v>279</v>
       </c>
@@ -20768,8 +20938,14 @@
       <c r="P63" s="1" t="s">
         <v>1104</v>
       </c>
-    </row>
-    <row r="64" spans="1:16">
+      <c r="Q63" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R63" s="1" t="s">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18">
       <c r="A64" s="1" t="s">
         <v>283</v>
       </c>
@@ -20814,6 +20990,12 @@
       </c>
       <c r="P64" s="1" t="s">
         <v>1104</v>
+      </c>
+      <c r="Q64" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R64" s="1" t="s">
+        <v>1325</v>
       </c>
     </row>
     <row r="65" spans="1:18">

</xml_diff>

<commit_message>
swap() added, tested. Opcodes table updated.
</commit_message>
<xml_diff>
--- a/other/op_codes_implementations.xlsx
+++ b/other/op_codes_implementations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="360" windowWidth="25940" windowHeight="16080" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="980" yWindow="360" windowWidth="25940" windowHeight="16080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Main Codes" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8710" uniqueCount="1326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8822" uniqueCount="1330">
   <si>
     <t>0</t>
   </si>
@@ -4051,6 +4051,18 @@
   </si>
   <si>
     <t>rotateRightThroughFlag(false)</t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>complement</t>
+  </si>
+  <si>
+    <t>swap</t>
+  </si>
+  <si>
+    <t>A.sub(n)</t>
   </si>
 </sst>
 </file>
@@ -4099,8 +4111,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4148,7 +4184,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="67">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4170,6 +4206,18 @@
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4191,6 +4239,18 @@
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4530,8 +4590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R256"/>
   <sheetViews>
-    <sheetView topLeftCell="A233" workbookViewId="0">
-      <selection activeCell="Q49" sqref="Q49"/>
+    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
+      <selection activeCell="R212" sqref="R212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4551,7 +4611,7 @@
     <col min="13" max="13" width="3.33203125" customWidth="1"/>
     <col min="14" max="14" width="3.1640625" customWidth="1"/>
     <col min="15" max="15" width="4.1640625" customWidth="1"/>
-    <col min="16" max="16" width="63.83203125" customWidth="1"/>
+    <col min="16" max="16" width="61.83203125" customWidth="1"/>
     <col min="17" max="17" width="12.83203125" customWidth="1"/>
     <col min="18" max="18" width="14.1640625" customWidth="1"/>
   </cols>
@@ -7105,6 +7165,12 @@
       <c r="P48" s="1" t="s">
         <v>228</v>
       </c>
+      <c r="Q48" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R48" s="1" t="s">
+        <v>1327</v>
+      </c>
     </row>
     <row r="49" spans="1:18">
       <c r="A49" s="1" t="s">
@@ -13288,7 +13354,7 @@
         <v>1314</v>
       </c>
     </row>
-    <row r="161" spans="1:16">
+    <row r="161" spans="1:18">
       <c r="A161" s="1" t="s">
         <v>619</v>
       </c>
@@ -13334,8 +13400,14 @@
       <c r="P161" s="1" t="s">
         <v>624</v>
       </c>
-    </row>
-    <row r="162" spans="1:16">
+      <c r="Q161" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R161" s="1" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="162" spans="1:18">
       <c r="A162" s="1" t="s">
         <v>625</v>
       </c>
@@ -13381,8 +13453,14 @@
       <c r="P162" s="1" t="s">
         <v>624</v>
       </c>
-    </row>
-    <row r="163" spans="1:16">
+      <c r="Q162" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R162" s="1" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="163" spans="1:18">
       <c r="A163" s="1" t="s">
         <v>629</v>
       </c>
@@ -13428,8 +13506,14 @@
       <c r="P163" s="1" t="s">
         <v>624</v>
       </c>
-    </row>
-    <row r="164" spans="1:16">
+      <c r="Q163" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R163" s="1" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="164" spans="1:18">
       <c r="A164" s="1" t="s">
         <v>633</v>
       </c>
@@ -13475,8 +13559,14 @@
       <c r="P164" s="1" t="s">
         <v>624</v>
       </c>
-    </row>
-    <row r="165" spans="1:16">
+      <c r="Q164" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R164" s="1" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="165" spans="1:18">
       <c r="A165" s="1" t="s">
         <v>637</v>
       </c>
@@ -13522,8 +13612,14 @@
       <c r="P165" s="1" t="s">
         <v>624</v>
       </c>
-    </row>
-    <row r="166" spans="1:16">
+      <c r="Q165" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R165" s="1" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="166" spans="1:18">
       <c r="A166" s="1" t="s">
         <v>641</v>
       </c>
@@ -13569,8 +13665,14 @@
       <c r="P166" s="1" t="s">
         <v>624</v>
       </c>
-    </row>
-    <row r="167" spans="1:16">
+      <c r="Q166" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R166" s="1" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="167" spans="1:18">
       <c r="A167" s="1" t="s">
         <v>645</v>
       </c>
@@ -13616,8 +13718,14 @@
       <c r="P167" s="1" t="s">
         <v>624</v>
       </c>
-    </row>
-    <row r="168" spans="1:16">
+      <c r="Q167" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R167" s="1" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="168" spans="1:18">
       <c r="A168" s="1" t="s">
         <v>649</v>
       </c>
@@ -13663,8 +13771,14 @@
       <c r="P168" s="1" t="s">
         <v>624</v>
       </c>
-    </row>
-    <row r="169" spans="1:16">
+      <c r="Q168" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R168" s="1" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="169" spans="1:18">
       <c r="A169" s="1" t="s">
         <v>653</v>
       </c>
@@ -13710,8 +13824,14 @@
       <c r="P169" s="1" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="170" spans="1:16">
+      <c r="Q169" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R169" s="1" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="170" spans="1:18">
       <c r="A170" s="1" t="s">
         <v>659</v>
       </c>
@@ -13757,8 +13877,14 @@
       <c r="P170" s="1" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="171" spans="1:16">
+      <c r="Q170" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R170" s="1" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="171" spans="1:18">
       <c r="A171" s="1" t="s">
         <v>663</v>
       </c>
@@ -13804,8 +13930,14 @@
       <c r="P171" s="1" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="172" spans="1:16">
+      <c r="Q171" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R171" s="1" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="172" spans="1:18">
       <c r="A172" s="1" t="s">
         <v>667</v>
       </c>
@@ -13851,8 +13983,14 @@
       <c r="P172" s="1" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="173" spans="1:16">
+      <c r="Q172" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R172" s="1" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="173" spans="1:18">
       <c r="A173" s="1" t="s">
         <v>671</v>
       </c>
@@ -13898,8 +14036,14 @@
       <c r="P173" s="1" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="174" spans="1:16">
+      <c r="Q173" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R173" s="1" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="174" spans="1:18">
       <c r="A174" s="1" t="s">
         <v>675</v>
       </c>
@@ -13945,8 +14089,14 @@
       <c r="P174" s="1" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="175" spans="1:16">
+      <c r="Q174" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R174" s="1" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="175" spans="1:18">
       <c r="A175" s="1" t="s">
         <v>679</v>
       </c>
@@ -13992,8 +14142,14 @@
       <c r="P175" s="1" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="176" spans="1:16">
+      <c r="Q175" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R175" s="1" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="176" spans="1:18">
       <c r="A176" s="1" t="s">
         <v>683</v>
       </c>
@@ -14039,8 +14195,14 @@
       <c r="P176" s="1" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="177" spans="1:16">
+      <c r="Q176" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R176" s="1" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="177" spans="1:18">
       <c r="A177" s="1" t="s">
         <v>687</v>
       </c>
@@ -14086,8 +14248,14 @@
       <c r="P177" s="1" t="s">
         <v>692</v>
       </c>
-    </row>
-    <row r="178" spans="1:16">
+      <c r="Q177" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R177" s="1" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="178" spans="1:18">
       <c r="A178" s="1" t="s">
         <v>693</v>
       </c>
@@ -14133,8 +14301,14 @@
       <c r="P178" s="1" t="s">
         <v>692</v>
       </c>
-    </row>
-    <row r="179" spans="1:16">
+      <c r="Q178" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R178" s="1" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="179" spans="1:18">
       <c r="A179" s="1" t="s">
         <v>697</v>
       </c>
@@ -14180,8 +14354,14 @@
       <c r="P179" s="1" t="s">
         <v>692</v>
       </c>
-    </row>
-    <row r="180" spans="1:16">
+      <c r="Q179" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R179" s="1" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="180" spans="1:18">
       <c r="A180" s="1" t="s">
         <v>701</v>
       </c>
@@ -14227,8 +14407,14 @@
       <c r="P180" s="1" t="s">
         <v>692</v>
       </c>
-    </row>
-    <row r="181" spans="1:16">
+      <c r="Q180" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R180" s="1" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="181" spans="1:18">
       <c r="A181" s="1" t="s">
         <v>705</v>
       </c>
@@ -14274,8 +14460,14 @@
       <c r="P181" s="1" t="s">
         <v>692</v>
       </c>
-    </row>
-    <row r="182" spans="1:16">
+      <c r="Q181" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R181" s="1" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="182" spans="1:18">
       <c r="A182" s="1" t="s">
         <v>709</v>
       </c>
@@ -14321,8 +14513,14 @@
       <c r="P182" s="1" t="s">
         <v>692</v>
       </c>
-    </row>
-    <row r="183" spans="1:16">
+      <c r="Q182" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R182" s="1" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="183" spans="1:18">
       <c r="A183" s="1" t="s">
         <v>713</v>
       </c>
@@ -14368,8 +14566,14 @@
       <c r="P183" s="1" t="s">
         <v>692</v>
       </c>
-    </row>
-    <row r="184" spans="1:16">
+      <c r="Q183" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R183" s="1" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="184" spans="1:18">
       <c r="A184" s="1" t="s">
         <v>717</v>
       </c>
@@ -14415,8 +14619,14 @@
       <c r="P184" s="1" t="s">
         <v>692</v>
       </c>
-    </row>
-    <row r="185" spans="1:16">
+      <c r="Q184" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R184" s="1" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="185" spans="1:18">
       <c r="A185" s="1" t="s">
         <v>721</v>
       </c>
@@ -14462,8 +14672,14 @@
       <c r="P185" s="1" t="s">
         <v>726</v>
       </c>
-    </row>
-    <row r="186" spans="1:16">
+      <c r="Q185" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R185" s="1" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="186" spans="1:18">
       <c r="A186" s="1" t="s">
         <v>727</v>
       </c>
@@ -14509,8 +14725,14 @@
       <c r="P186" s="1" t="s">
         <v>726</v>
       </c>
-    </row>
-    <row r="187" spans="1:16">
+      <c r="Q186" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R186" s="1" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="187" spans="1:18">
       <c r="A187" s="1" t="s">
         <v>731</v>
       </c>
@@ -14556,8 +14778,14 @@
       <c r="P187" s="1" t="s">
         <v>726</v>
       </c>
-    </row>
-    <row r="188" spans="1:16">
+      <c r="Q187" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R187" s="1" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="188" spans="1:18">
       <c r="A188" s="1" t="s">
         <v>735</v>
       </c>
@@ -14603,8 +14831,14 @@
       <c r="P188" s="1" t="s">
         <v>726</v>
       </c>
-    </row>
-    <row r="189" spans="1:16">
+      <c r="Q188" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R188" s="1" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="189" spans="1:18">
       <c r="A189" s="1" t="s">
         <v>739</v>
       </c>
@@ -14650,8 +14884,14 @@
       <c r="P189" s="1" t="s">
         <v>726</v>
       </c>
-    </row>
-    <row r="190" spans="1:16">
+      <c r="Q189" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R189" s="1" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="190" spans="1:18">
       <c r="A190" s="1" t="s">
         <v>742</v>
       </c>
@@ -14697,8 +14937,14 @@
       <c r="P190" s="1" t="s">
         <v>726</v>
       </c>
-    </row>
-    <row r="191" spans="1:16">
+      <c r="Q190" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R190" s="1" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="191" spans="1:18">
       <c r="A191" s="1" t="s">
         <v>746</v>
       </c>
@@ -14744,8 +14990,14 @@
       <c r="P191" s="1" t="s">
         <v>726</v>
       </c>
-    </row>
-    <row r="192" spans="1:16">
+      <c r="Q191" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R191" s="1" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="192" spans="1:18">
       <c r="A192" s="1" t="s">
         <v>750</v>
       </c>
@@ -14790,6 +15042,12 @@
       </c>
       <c r="P192" s="1" t="s">
         <v>726</v>
+      </c>
+      <c r="Q192" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R192" s="1" t="s">
+        <v>1329</v>
       </c>
     </row>
     <row r="193" spans="1:18">
@@ -15731,6 +15989,12 @@
       <c r="F212" s="1" t="s">
         <v>851</v>
       </c>
+      <c r="Q212" s="1" t="s">
+        <v>1326</v>
+      </c>
+      <c r="R212" s="1" t="s">
+        <v>1326</v>
+      </c>
     </row>
     <row r="213" spans="1:18">
       <c r="A213" s="1" t="s">
@@ -16089,6 +16353,12 @@
       <c r="F220" s="1" t="s">
         <v>851</v>
       </c>
+      <c r="Q220" s="1" t="s">
+        <v>1326</v>
+      </c>
+      <c r="R220" s="1" t="s">
+        <v>1326</v>
+      </c>
     </row>
     <row r="221" spans="1:18">
       <c r="A221" s="1" t="s">
@@ -16159,6 +16429,12 @@
       <c r="F222" s="1" t="s">
         <v>851</v>
       </c>
+      <c r="Q222" s="1" t="s">
+        <v>1326</v>
+      </c>
+      <c r="R222" s="1" t="s">
+        <v>1326</v>
+      </c>
     </row>
     <row r="223" spans="1:18">
       <c r="A223" s="1" t="s">
@@ -16435,6 +16711,12 @@
       <c r="F228" s="1" t="s">
         <v>851</v>
       </c>
+      <c r="Q228" s="1" t="s">
+        <v>1326</v>
+      </c>
+      <c r="R228" s="1" t="s">
+        <v>1326</v>
+      </c>
     </row>
     <row r="229" spans="1:18">
       <c r="A229" s="1" t="s">
@@ -16455,6 +16737,12 @@
       <c r="F229" s="1" t="s">
         <v>851</v>
       </c>
+      <c r="Q229" s="1" t="s">
+        <v>1326</v>
+      </c>
+      <c r="R229" s="1" t="s">
+        <v>1326</v>
+      </c>
     </row>
     <row r="230" spans="1:18">
       <c r="A230" s="1" t="s">
@@ -16549,6 +16837,12 @@
       <c r="P231" s="1" t="s">
         <v>624</v>
       </c>
+      <c r="Q231" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R231" s="1" t="s">
+        <v>623</v>
+      </c>
     </row>
     <row r="232" spans="1:18">
       <c r="A232" s="1" t="s">
@@ -16775,6 +17069,12 @@
       <c r="F236" s="1" t="s">
         <v>851</v>
       </c>
+      <c r="Q236" s="1" t="s">
+        <v>1326</v>
+      </c>
+      <c r="R236" s="1" t="s">
+        <v>1326</v>
+      </c>
     </row>
     <row r="237" spans="1:18">
       <c r="A237" s="1" t="s">
@@ -16795,6 +17095,12 @@
       <c r="F237" s="1" t="s">
         <v>851</v>
       </c>
+      <c r="Q237" s="1" t="s">
+        <v>1326</v>
+      </c>
+      <c r="R237" s="1" t="s">
+        <v>1326</v>
+      </c>
     </row>
     <row r="238" spans="1:18">
       <c r="A238" s="1" t="s">
@@ -16815,6 +17121,12 @@
       <c r="F238" s="1" t="s">
         <v>851</v>
       </c>
+      <c r="Q238" s="1" t="s">
+        <v>1326</v>
+      </c>
+      <c r="R238" s="1" t="s">
+        <v>1326</v>
+      </c>
     </row>
     <row r="239" spans="1:18">
       <c r="A239" s="1" t="s">
@@ -16862,6 +17174,12 @@
       <c r="P239" s="1" t="s">
         <v>658</v>
       </c>
+      <c r="Q239" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R239" s="1" t="s">
+        <v>657</v>
+      </c>
     </row>
     <row r="240" spans="1:18">
       <c r="A240" s="1" t="s">
@@ -16959,6 +17277,12 @@
       <c r="P241" s="1" t="s">
         <v>906</v>
       </c>
+      <c r="Q241" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R241" s="1" t="s">
+        <v>1312</v>
+      </c>
     </row>
     <row r="242" spans="1:18">
       <c r="A242" s="1" t="s">
@@ -17126,6 +17450,12 @@
       <c r="F245" s="1" t="s">
         <v>851</v>
       </c>
+      <c r="Q245" s="1" t="s">
+        <v>1326</v>
+      </c>
+      <c r="R245" s="1" t="s">
+        <v>1326</v>
+      </c>
     </row>
     <row r="246" spans="1:18">
       <c r="A246" s="1" t="s">
@@ -17220,6 +17550,12 @@
       <c r="P247" s="1" t="s">
         <v>692</v>
       </c>
+      <c r="Q247" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R247" s="1" t="s">
+        <v>691</v>
+      </c>
     </row>
     <row r="248" spans="1:18">
       <c r="A248" s="1" t="s">
@@ -17499,6 +17835,12 @@
       <c r="F253" s="1" t="s">
         <v>851</v>
       </c>
+      <c r="Q253" s="1" t="s">
+        <v>1326</v>
+      </c>
+      <c r="R253" s="1" t="s">
+        <v>1326</v>
+      </c>
     </row>
     <row r="254" spans="1:18">
       <c r="A254" s="1" t="s">
@@ -17518,6 +17860,12 @@
       </c>
       <c r="F254" s="1" t="s">
         <v>851</v>
+      </c>
+      <c r="Q254" s="1" t="s">
+        <v>1326</v>
+      </c>
+      <c r="R254" s="1" t="s">
+        <v>1326</v>
       </c>
     </row>
     <row r="255" spans="1:18">
@@ -17629,8 +17977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A225" workbookViewId="0">
-      <selection activeCell="R53" sqref="R53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R49" sqref="R49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -17650,8 +17998,8 @@
     <col min="13" max="13" width="2.5" customWidth="1"/>
     <col min="14" max="14" width="3" customWidth="1"/>
     <col min="15" max="15" width="3.33203125" customWidth="1"/>
-    <col min="16" max="16" width="36.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="24" customWidth="1"/>
+    <col min="16" max="16" width="38.83203125" customWidth="1"/>
+    <col min="18" max="18" width="34.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -20244,6 +20592,12 @@
       <c r="P49" s="1" t="s">
         <v>1094</v>
       </c>
+      <c r="Q49" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R49" s="1" t="s">
+        <v>1328</v>
+      </c>
     </row>
     <row r="50" spans="1:18">
       <c r="A50" s="1" t="s">
@@ -20291,6 +20645,12 @@
       <c r="P50" s="1" t="s">
         <v>1094</v>
       </c>
+      <c r="Q50" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R50" s="1" t="s">
+        <v>1328</v>
+      </c>
     </row>
     <row r="51" spans="1:18">
       <c r="A51" s="1" t="s">
@@ -20338,6 +20698,12 @@
       <c r="P51" s="1" t="s">
         <v>1094</v>
       </c>
+      <c r="Q51" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R51" s="1" t="s">
+        <v>1328</v>
+      </c>
     </row>
     <row r="52" spans="1:18">
       <c r="A52" s="1" t="s">
@@ -20385,6 +20751,12 @@
       <c r="P52" s="1" t="s">
         <v>1094</v>
       </c>
+      <c r="Q52" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R52" s="1" t="s">
+        <v>1328</v>
+      </c>
     </row>
     <row r="53" spans="1:18">
       <c r="A53" s="1" t="s">
@@ -20432,6 +20804,12 @@
       <c r="P53" s="1" t="s">
         <v>1094</v>
       </c>
+      <c r="Q53" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R53" s="1" t="s">
+        <v>1328</v>
+      </c>
     </row>
     <row r="54" spans="1:18">
       <c r="A54" s="1" t="s">
@@ -20479,6 +20857,12 @@
       <c r="P54" s="1" t="s">
         <v>1094</v>
       </c>
+      <c r="Q54" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R54" s="1" t="s">
+        <v>1328</v>
+      </c>
     </row>
     <row r="55" spans="1:18">
       <c r="A55" s="1" t="s">
@@ -20526,6 +20910,12 @@
       <c r="P55" s="1" t="s">
         <v>1094</v>
       </c>
+      <c r="Q55" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R55" s="1" t="s">
+        <v>1328</v>
+      </c>
     </row>
     <row r="56" spans="1:18">
       <c r="A56" s="1" t="s">
@@ -20572,6 +20962,12 @@
       </c>
       <c r="P56" s="1" t="s">
         <v>1094</v>
+      </c>
+      <c r="Q56" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="R56" s="1" t="s">
+        <v>1328</v>
       </c>
     </row>
     <row r="57" spans="1:18">

</xml_diff>

<commit_message>
Interim commit, changes to opcode implementation table.
</commit_message>
<xml_diff>
--- a/other/op_codes_implementations.xlsx
+++ b/other/op_codes_implementations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="360" windowWidth="25940" windowHeight="16080" tabRatio="500"/>
+    <workbookView xWindow="6380" yWindow="1100" windowWidth="27060" windowHeight="16080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Main Codes" sheetId="1" r:id="rId1"/>
@@ -4590,8 +4590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
-      <selection activeCell="R212" sqref="R212"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="Q223" sqref="Q223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>